<commit_message>
Add Amp Driver Manual
Add Amp Driver Manual
</commit_message>
<xml_diff>
--- a/K9HZ_KI3P_Amp_Driver/K9HZ_KI3P_Amp_Driver_BOM_010225.xlsx
+++ b/K9HZ_KI3P_Amp_Driver/K9HZ_KI3P_Amp_Driver_BOM_010225.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dad\Documents\GitHub\K9HZ\K9HZ_KI3P_Amp_Driver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dad\Documents\GitHub\K9HZ_KI3P\K9HZ_KI3P_Amp_Driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A647E0B3-B5DA-4D4D-8E37-2496B6AED195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA205B21-B433-4DC8-AC37-3CB91C396473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EDED857D-3C86-4F60-A9F1-02B0562F0948}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Qty</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Digikey</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>Tayda Electronics</t>
   </si>
   <si>
@@ -138,21 +135,12 @@
   </si>
   <si>
     <t>A-2115</t>
-  </si>
-  <si>
-    <t>Shipping</t>
-  </si>
-  <si>
-    <t>Tot Parts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -304,7 +292,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -484,14 +472,8 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -606,17 +588,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -659,9 +632,8 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -673,17 +645,8 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1"/>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="19" fillId="33" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -711,7 +674,6 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Currency" xfId="42" builtinId="4"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -1058,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD02558-313C-4E06-BB6D-69026BD3D1AD}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -1075,7 +1037,7 @@
     <col min="7" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1092,19 +1054,10 @@
         <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>2</v>
       </c>
@@ -1115,21 +1068,10 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0.06</v>
-      </c>
-      <c r="H2" s="6">
-        <f>A2*G2</f>
-        <v>0.12</v>
-      </c>
-      <c r="I2" s="5">
-        <f>A2*0.02</f>
-        <v>0.04</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1140,21 +1082,10 @@
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0.04</v>
-      </c>
-      <c r="H3" s="6">
-        <f t="shared" ref="H3:H10" si="0">A3*G3</f>
-        <v>0.04</v>
-      </c>
-      <c r="I3" s="5">
-        <f t="shared" ref="I3:I10" si="1">A3*0.02</f>
-        <v>0.02</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1162,24 +1093,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0.04</v>
-      </c>
-      <c r="H4" s="6">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
-      </c>
-      <c r="I4" s="5">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -1187,24 +1107,13 @@
         <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0.04</v>
-      </c>
-      <c r="H5" s="6">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
-      </c>
-      <c r="I5" s="5">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -1217,19 +1126,8 @@
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="10">
-        <v>0.71</v>
-      </c>
-      <c r="H6" s="11">
-        <f t="shared" si="0"/>
-        <v>0.71</v>
-      </c>
-      <c r="I6" s="10">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -1237,27 +1135,16 @@
         <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0.12</v>
-      </c>
-      <c r="H7" s="6">
-        <f t="shared" si="0"/>
-        <v>0.12</v>
-      </c>
-      <c r="I7" s="5">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>2</v>
       </c>
@@ -1268,21 +1155,10 @@
         <v>14</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1.2E-2</v>
-      </c>
-      <c r="H8" s="6">
-        <f t="shared" si="0"/>
-        <v>2.4E-2</v>
-      </c>
-      <c r="I8" s="5">
-        <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -1293,21 +1169,10 @@
         <v>16</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1.2E-2</v>
-      </c>
-      <c r="H9" s="6">
-        <f t="shared" si="0"/>
-        <v>1.2E-2</v>
-      </c>
-      <c r="I9" s="5">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -1317,36 +1182,8 @@
       <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="5">
-        <f>0.3</f>
-        <v>0.3</v>
-      </c>
-      <c r="H10" s="7">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
-      <c r="I10" s="9">
-        <v>0.2</v>
-      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="G11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="6">
-        <f>SUM(H2:H10)</f>
-        <v>1.4059999999999999</v>
-      </c>
-      <c r="I11" s="5">
-        <f>SUM(I2:I10)</f>
-        <v>0.4</v>
-      </c>
-      <c r="J11" s="6">
-        <f>H11+I11</f>
-        <v>1.806</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>

</xml_diff>